<commit_message>
data collection for the manuscript
</commit_message>
<xml_diff>
--- a/Matlab/Simscape models/Graphs/draft7/Ligament Properties.xlsx
+++ b/Matlab/Simscape models/Graphs/draft7/Ligament Properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siril\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siril\OneDrive\Desktop\TIM-Control\Matlab\Simscape models\Graphs\draft7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B356BE-9E71-4E4D-8139-FE778E755883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F14B518-2F6B-4077-9766-D7E9C0AAE209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{D3468EB1-82D2-459F-84A7-81333EBF17E9}"/>
+    <workbookView xWindow="29604" yWindow="13008" windowWidth="11712" windowHeight="13776" xr2:uid="{D3468EB1-82D2-459F-84A7-81333EBF17E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="61">
   <si>
     <t>Bi-linear</t>
   </si>
@@ -197,6 +197,36 @@
   <si>
     <t>Force - displacement curves of Intertransverse ligaments (x 4 springs on each side)</t>
   </si>
+  <si>
+    <t>For the manuscript</t>
+  </si>
+  <si>
+    <t>ISL</t>
+  </si>
+  <si>
+    <t>SSL</t>
+  </si>
+  <si>
+    <t>ITL</t>
+  </si>
+  <si>
+    <t>E (Mpa) - From Eberlin</t>
+  </si>
+  <si>
+    <t>* per side</t>
+  </si>
+  <si>
+    <t>12*</t>
+  </si>
+  <si>
+    <t>4*</t>
+  </si>
+  <si>
+    <t>no of spring elements - Shirazi 1986</t>
+  </si>
+  <si>
+    <t>Area (mm^2) - from Shirazi Adl 1986</t>
+  </si>
 </sst>
 </file>
 
@@ -249,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -309,11 +339,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -354,17 +464,8 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -382,20 +483,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -404,12 +496,48 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4296,8 +4424,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>380429</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>5485</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>14450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4758,25 +4886,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68065608-4F08-4037-B003-A33791418087}">
-  <dimension ref="B1:AP34"/>
+  <dimension ref="B1:AP44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE34" sqref="AE34"/>
+    <sheetView tabSelected="1" topLeftCell="AD24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ48" sqref="AJ48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.28515625" customWidth="1"/>
-    <col min="19" max="20" width="17.140625" customWidth="1"/>
-    <col min="21" max="21" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" customWidth="1"/>
+    <col min="16" max="16" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" customWidth="1"/>
+    <col min="19" max="20" width="17.109375" customWidth="1"/>
+    <col min="21" max="21" width="21.109375" customWidth="1"/>
+    <col min="34" max="34" width="21.6640625" customWidth="1"/>
+    <col min="35" max="35" width="18.5546875" customWidth="1"/>
+    <col min="36" max="36" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4793,7 +4924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
@@ -4836,10 +4967,10 @@
       <c r="S2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="T2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="U2" s="16"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="7" t="s">
         <v>10</v>
       </c>
@@ -4867,33 +4998,33 @@
       <c r="AD2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AG2" s="29" t="s">
+      <c r="AG2" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="AH2" s="29"/>
-      <c r="AI2" s="29"/>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="29"/>
-      <c r="AL2" s="29"/>
-      <c r="AM2" s="29"/>
-      <c r="AN2" s="29"/>
-      <c r="AO2" s="29"/>
-      <c r="AP2" s="29"/>
+      <c r="AH2" s="30"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="30"/>
+      <c r="AK2" s="30"/>
+      <c r="AL2" s="30"/>
+      <c r="AM2" s="30"/>
+      <c r="AN2" s="30"/>
+      <c r="AO2" s="30"/>
+      <c r="AP2" s="30"/>
     </row>
-    <row r="3" spans="2:42" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:42" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="31">
         <v>3</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="31">
         <v>25.2</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="32" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="1">
@@ -4915,25 +5046,25 @@
         <f>((15/D3*E3/G3)*(J3-H3)+I3)</f>
         <v>114.24</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="25" t="s">
+      <c r="Q3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="26">
+      <c r="R3" s="33">
         <v>3</v>
       </c>
-      <c r="S3" s="26">
+      <c r="S3" s="33">
         <v>25.2</v>
       </c>
-      <c r="T3" s="25" t="s">
+      <c r="T3" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="U3" s="25" t="s">
+      <c r="U3" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="V3" s="27">
+      <c r="V3" s="23">
         <v>27.2</v>
       </c>
       <c r="W3" s="14">
@@ -4968,35 +5099,35 @@
         <f>$U$7*$S$3/$R$3</f>
         <v>84</v>
       </c>
-      <c r="AG3" s="30" t="s">
+      <c r="AG3" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="AH3" s="30"/>
-      <c r="AI3" s="30" t="s">
+      <c r="AH3" s="29"/>
+      <c r="AI3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="AJ3" s="30"/>
-      <c r="AK3" s="30" t="s">
+      <c r="AJ3" s="29"/>
+      <c r="AK3" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="AL3" s="30"/>
-      <c r="AM3" s="30" t="s">
+      <c r="AL3" s="29"/>
+      <c r="AM3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="AN3" s="30"/>
-      <c r="AO3" s="30" t="s">
+      <c r="AN3" s="29"/>
+      <c r="AO3" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="AP3" s="30"/>
+      <c r="AP3" s="29"/>
     </row>
-    <row r="4" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="1">
         <v>22.3</v>
       </c>
@@ -5022,19 +5153,19 @@
       <c r="N4">
         <v>342.72</v>
       </c>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="25" t="s">
+      <c r="P4" s="21"/>
+      <c r="Q4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="25">
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="22">
         <v>0.01</v>
       </c>
-      <c r="U4" s="28">
+      <c r="U4" s="24">
         <v>0</v>
       </c>
-      <c r="V4" s="27">
+      <c r="V4" s="23">
         <v>22.3</v>
       </c>
       <c r="W4" s="14">
@@ -5069,45 +5200,45 @@
         <f t="shared" ref="AD4:AD7" si="8">$U$7*$S$3/$R$3</f>
         <v>84</v>
       </c>
-      <c r="AG4" s="31" t="s">
+      <c r="AG4" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AH4" s="31" t="s">
+      <c r="AH4" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AI4" s="31" t="s">
+      <c r="AI4" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AJ4" s="31" t="s">
+      <c r="AJ4" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AK4" s="31" t="s">
+      <c r="AK4" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AL4" s="31" t="s">
+      <c r="AL4" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AM4" s="31" t="s">
+      <c r="AM4" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AN4" s="31" t="s">
+      <c r="AN4" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AO4" s="31" t="s">
+      <c r="AO4" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AP4" s="31" t="s">
+      <c r="AP4" s="25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="1">
         <v>19.399999999999999</v>
       </c>
@@ -5127,19 +5258,19 @@
         <f>((15/D3*E3/G5)*(J5-H5)+I5)</f>
         <v>114.24000000000001</v>
       </c>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="25" t="s">
+      <c r="P5" s="21"/>
+      <c r="Q5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="25">
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="22">
         <v>0.15</v>
       </c>
-      <c r="U5" s="28">
+      <c r="U5" s="24">
         <v>1</v>
       </c>
-      <c r="V5" s="27">
+      <c r="V5" s="23">
         <v>19.399999999999999</v>
       </c>
       <c r="W5" s="14">
@@ -5174,45 +5305,45 @@
         <f t="shared" si="8"/>
         <v>84</v>
       </c>
-      <c r="AG5" s="31">
+      <c r="AG5" s="25">
         <v>0.27200000000000002</v>
       </c>
-      <c r="AH5" s="31">
+      <c r="AH5" s="25">
         <v>0</v>
       </c>
-      <c r="AI5" s="31">
+      <c r="AI5" s="25">
         <v>0.223</v>
       </c>
-      <c r="AJ5" s="31">
+      <c r="AJ5" s="25">
         <v>0</v>
       </c>
-      <c r="AK5" s="31">
+      <c r="AK5" s="25">
         <v>0.19399999999999998</v>
       </c>
-      <c r="AL5" s="31">
+      <c r="AL5" s="25">
         <v>0</v>
       </c>
-      <c r="AM5" s="31">
+      <c r="AM5" s="25">
         <v>0.26800000000000002</v>
       </c>
-      <c r="AN5" s="31">
+      <c r="AN5" s="25">
         <v>0</v>
       </c>
-      <c r="AO5" s="31">
+      <c r="AO5" s="25">
         <v>0.223</v>
       </c>
-      <c r="AP5" s="31">
+      <c r="AP5" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="1">
         <v>26.8</v>
       </c>
@@ -5232,19 +5363,19 @@
         <f>((15/D3*E3/G6)*(J6-H6)+I6)</f>
         <v>114.24000000000001</v>
       </c>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="25" t="s">
+      <c r="P6" s="21"/>
+      <c r="Q6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="25">
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="22">
         <v>0.22</v>
       </c>
-      <c r="U6" s="28">
+      <c r="U6" s="24">
         <v>2.5</v>
       </c>
-      <c r="V6" s="27">
+      <c r="V6" s="23">
         <v>26.8</v>
       </c>
       <c r="W6" s="14">
@@ -5279,45 +5410,45 @@
         <f t="shared" si="8"/>
         <v>84</v>
       </c>
-      <c r="AG6" s="31">
+      <c r="AG6" s="25">
         <v>4.08</v>
       </c>
-      <c r="AH6" s="31">
+      <c r="AH6" s="25">
         <v>8.4</v>
       </c>
-      <c r="AI6" s="31">
+      <c r="AI6" s="25">
         <v>3.3450000000000002</v>
       </c>
-      <c r="AJ6" s="31">
+      <c r="AJ6" s="25">
         <v>8.4</v>
       </c>
-      <c r="AK6" s="31">
+      <c r="AK6" s="25">
         <v>2.9099999999999997</v>
       </c>
-      <c r="AL6" s="31">
+      <c r="AL6" s="25">
         <v>8.4</v>
       </c>
-      <c r="AM6" s="31">
+      <c r="AM6" s="25">
         <v>4.0199999999999996</v>
       </c>
-      <c r="AN6" s="31">
+      <c r="AN6" s="25">
         <v>8.4</v>
       </c>
-      <c r="AO6" s="31">
+      <c r="AO6" s="25">
         <v>3.3450000000000002</v>
       </c>
-      <c r="AP6" s="31">
+      <c r="AP6" s="25">
         <v>8.4</v>
       </c>
     </row>
-    <row r="7" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="1">
         <v>22.3</v>
       </c>
@@ -5337,19 +5468,19 @@
         <f>((15/$D$3*$E$3/G7)*(J7-H7)+I7)</f>
         <v>114.23999999999998</v>
       </c>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="25" t="s">
+      <c r="P7" s="21"/>
+      <c r="Q7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="25">
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="22">
         <v>0.28999999999999998</v>
       </c>
-      <c r="U7" s="28">
+      <c r="U7" s="24">
         <v>10</v>
       </c>
-      <c r="V7" s="27">
+      <c r="V7" s="23">
         <v>22.3</v>
       </c>
       <c r="W7" s="14">
@@ -5384,51 +5515,51 @@
         <f t="shared" si="8"/>
         <v>84</v>
       </c>
-      <c r="AG7" s="31">
+      <c r="AG7" s="25">
         <v>5.984</v>
       </c>
-      <c r="AH7" s="31">
+      <c r="AH7" s="25">
         <v>21</v>
       </c>
-      <c r="AI7" s="31">
+      <c r="AI7" s="25">
         <v>4.9060000000000006</v>
       </c>
-      <c r="AJ7" s="31">
+      <c r="AJ7" s="25">
         <v>21</v>
       </c>
-      <c r="AK7" s="31">
+      <c r="AK7" s="25">
         <v>4.2679999999999998</v>
       </c>
-      <c r="AL7" s="31">
+      <c r="AL7" s="25">
         <v>21</v>
       </c>
-      <c r="AM7" s="31">
+      <c r="AM7" s="25">
         <v>5.8959999999999999</v>
       </c>
-      <c r="AN7" s="31">
+      <c r="AN7" s="25">
         <v>21</v>
       </c>
-      <c r="AO7" s="31">
+      <c r="AO7" s="25">
         <v>4.9060000000000006</v>
       </c>
-      <c r="AP7" s="31">
+      <c r="AP7" s="25">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="31">
         <v>4</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="31">
         <v>35.1</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="32" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="1">
@@ -5450,25 +5581,25 @@
         <f>((11.6/$D$8*$E$8/G8)*(J8-H8)+I8)</f>
         <v>99.824400000000011</v>
       </c>
-      <c r="P8" s="18" t="s">
+      <c r="P8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="Q8" s="19" t="s">
+      <c r="Q8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="R8" s="20">
+      <c r="R8" s="34">
         <v>4</v>
       </c>
-      <c r="S8" s="20">
+      <c r="S8" s="34">
         <v>35.1</v>
       </c>
-      <c r="T8" s="19" t="s">
+      <c r="T8" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="U8" s="19" t="s">
+      <c r="U8" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="V8" s="21">
+      <c r="V8" s="18">
         <v>18.02</v>
       </c>
       <c r="W8" s="14">
@@ -5503,44 +5634,44 @@
         <f>$U$12*$S$8/$R$8</f>
         <v>48.262500000000003</v>
       </c>
-      <c r="AG8" s="31">
+      <c r="AG8" s="25">
         <v>7.887999999999999</v>
       </c>
-      <c r="AH8" s="31">
+      <c r="AH8" s="25">
         <v>84</v>
       </c>
-      <c r="AI8" s="31">
+      <c r="AI8" s="25">
         <v>6.4669999999999996</v>
       </c>
-      <c r="AJ8" s="31">
+      <c r="AJ8" s="25">
         <v>84</v>
       </c>
-      <c r="AK8" s="31">
+      <c r="AK8" s="25">
         <v>5.6259999999999994</v>
       </c>
-      <c r="AL8" s="31">
+      <c r="AL8" s="25">
         <v>84</v>
       </c>
-      <c r="AM8" s="31">
+      <c r="AM8" s="25">
         <v>7.7719999999999994</v>
       </c>
-      <c r="AN8" s="31">
+      <c r="AN8" s="25">
         <v>84</v>
       </c>
-      <c r="AO8" s="31">
+      <c r="AO8" s="25">
         <v>6.4669999999999996</v>
       </c>
-      <c r="AP8" s="31">
+      <c r="AP8" s="25">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:42" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="1">
         <v>10.3</v>
       </c>
@@ -5560,19 +5691,19 @@
         <f t="shared" ref="K9:K12" si="12">((11.6/$D$8*$E$8/G9)*(J9-H9)+I9)</f>
         <v>99.824400000000011</v>
       </c>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="19" t="s">
+      <c r="P9" s="19"/>
+      <c r="Q9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="19">
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="17">
         <v>0.01</v>
       </c>
-      <c r="U9" s="23">
+      <c r="U9" s="20">
         <v>0</v>
       </c>
-      <c r="V9" s="21">
+      <c r="V9" s="18">
         <v>10.3</v>
       </c>
       <c r="W9" s="14">
@@ -5608,13 +5739,13 @@
         <v>48.262500000000003</v>
       </c>
     </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:42" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="1">
         <v>5.4</v>
       </c>
@@ -5634,19 +5765,19 @@
         <f t="shared" si="12"/>
         <v>99.824400000000011</v>
       </c>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="19" t="s">
+      <c r="P10" s="19"/>
+      <c r="Q10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="19">
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="17">
         <v>0.1</v>
       </c>
-      <c r="U10" s="23">
+      <c r="U10" s="20">
         <v>0.55000000000000004</v>
       </c>
-      <c r="V10" s="21">
+      <c r="V10" s="18">
         <v>5.4</v>
       </c>
       <c r="W10" s="14">
@@ -5682,13 +5813,13 @@
         <v>48.262500000000003</v>
       </c>
     </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:42" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="1">
         <v>7.1</v>
       </c>
@@ -5708,19 +5839,19 @@
         <f t="shared" si="12"/>
         <v>99.824399999999997</v>
       </c>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="19" t="s">
+      <c r="P11" s="19"/>
+      <c r="Q11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="19">
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="17">
         <v>0.2</v>
       </c>
-      <c r="U11" s="23">
+      <c r="U11" s="20">
         <v>1.2</v>
       </c>
-      <c r="V11" s="21">
+      <c r="V11" s="18">
         <v>7.1</v>
       </c>
       <c r="W11" s="14">
@@ -5756,13 +5887,13 @@
         <v>48.262500000000003</v>
       </c>
     </row>
-    <row r="12" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
       <c r="G12" s="1">
         <v>10.5</v>
       </c>
@@ -5782,19 +5913,19 @@
         <f t="shared" si="12"/>
         <v>99.824399999999997</v>
       </c>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="19" t="s">
+      <c r="P12" s="19"/>
+      <c r="Q12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="19">
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="17">
         <v>0.6</v>
       </c>
-      <c r="U12" s="23">
+      <c r="U12" s="20">
         <v>5.5</v>
       </c>
-      <c r="V12" s="21">
+      <c r="V12" s="18">
         <v>10.5</v>
       </c>
       <c r="W12" s="14">
@@ -5833,20 +5964,20 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="31">
         <v>4</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="31">
         <v>12</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="32" t="s">
         <v>25</v>
       </c>
       <c r="G13" s="1">
@@ -5868,25 +5999,25 @@
         <f>((58.7/$D$13*$E$13/G13)*(J13-H13)+I13)</f>
         <v>149.80200000000002</v>
       </c>
-      <c r="P13" s="32" t="s">
+      <c r="P13" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="Q13" s="33" t="s">
+      <c r="Q13" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="R13" s="34">
+      <c r="R13" s="35">
         <v>4</v>
       </c>
-      <c r="S13" s="34">
+      <c r="S13" s="35">
         <v>12</v>
       </c>
-      <c r="T13" s="33" t="s">
+      <c r="T13" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="U13" s="33" t="s">
+      <c r="U13" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="V13" s="35">
+      <c r="V13" s="28">
         <v>17.8</v>
       </c>
       <c r="W13" s="14">
@@ -5921,29 +6052,29 @@
         <f>$U$17*$S$13/$R$13</f>
         <v>30</v>
       </c>
-      <c r="AG13" s="29" t="s">
+      <c r="AG13" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="AH13" s="29"/>
-      <c r="AI13" s="29"/>
-      <c r="AJ13" s="29"/>
-      <c r="AK13" s="29"/>
-      <c r="AL13" s="29"/>
-      <c r="AM13" s="29"/>
-      <c r="AN13" s="29"/>
-      <c r="AO13" s="29"/>
-      <c r="AP13" s="29"/>
+      <c r="AH13" s="30"/>
+      <c r="AI13" s="30"/>
+      <c r="AJ13" s="30"/>
+      <c r="AK13" s="30"/>
+      <c r="AL13" s="30"/>
+      <c r="AM13" s="30"/>
+      <c r="AN13" s="30"/>
+      <c r="AO13" s="30"/>
+      <c r="AP13" s="30"/>
     </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
       <c r="G14" s="1">
         <v>21.3</v>
       </c>
@@ -5963,21 +6094,21 @@
         <f t="shared" ref="K14:K17" si="23">((58.7/$D$13*$E$13/G14)*(J14-H14)+I14)</f>
         <v>149.80200000000002</v>
       </c>
-      <c r="P14" s="32" t="s">
+      <c r="P14" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="Q14" s="33" t="s">
+      <c r="Q14" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="R14" s="34"/>
-      <c r="S14" s="34"/>
-      <c r="T14" s="33">
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="27">
         <v>0.01</v>
       </c>
-      <c r="U14" s="33">
+      <c r="U14" s="27">
         <v>0</v>
       </c>
-      <c r="V14" s="35">
+      <c r="V14" s="28">
         <v>21.3</v>
       </c>
       <c r="W14" s="14">
@@ -6012,35 +6143,35 @@
         <f t="shared" ref="AD14:AD16" si="31">$U$17*$S$13/$R$13</f>
         <v>30</v>
       </c>
-      <c r="AG14" s="30" t="s">
+      <c r="AG14" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="AH14" s="30"/>
-      <c r="AI14" s="30" t="s">
+      <c r="AH14" s="29"/>
+      <c r="AI14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="AJ14" s="30"/>
-      <c r="AK14" s="30" t="s">
+      <c r="AJ14" s="29"/>
+      <c r="AK14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="AL14" s="30"/>
-      <c r="AM14" s="30" t="s">
+      <c r="AL14" s="29"/>
+      <c r="AM14" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="AN14" s="30"/>
-      <c r="AO14" s="30" t="s">
+      <c r="AN14" s="29"/>
+      <c r="AO14" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="AP14" s="30"/>
+      <c r="AP14" s="29"/>
     </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
       <c r="G15" s="1">
         <v>19.850000000000001</v>
       </c>
@@ -6060,19 +6191,19 @@
         <f t="shared" si="23"/>
         <v>149.80200000000002</v>
       </c>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="33" t="s">
+      <c r="P15" s="26"/>
+      <c r="Q15" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="R15" s="34"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="33">
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="27">
         <v>0.15</v>
       </c>
-      <c r="U15" s="33">
+      <c r="U15" s="27">
         <v>1</v>
       </c>
-      <c r="V15" s="35">
+      <c r="V15" s="28">
         <v>19.850000000000001</v>
       </c>
       <c r="W15" s="14">
@@ -6107,45 +6238,45 @@
         <f t="shared" si="31"/>
         <v>30</v>
       </c>
-      <c r="AG15" s="31" t="s">
+      <c r="AG15" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AH15" s="31" t="s">
+      <c r="AH15" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AI15" s="31" t="s">
+      <c r="AI15" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AJ15" s="31" t="s">
+      <c r="AJ15" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AK15" s="31" t="s">
+      <c r="AK15" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AL15" s="31" t="s">
+      <c r="AL15" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AM15" s="31" t="s">
+      <c r="AM15" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AN15" s="31" t="s">
+      <c r="AN15" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AO15" s="31" t="s">
+      <c r="AO15" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AP15" s="31" t="s">
+      <c r="AP15" s="25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
       <c r="G16" s="1">
         <v>20.84</v>
       </c>
@@ -6165,19 +6296,19 @@
         <f t="shared" si="23"/>
         <v>149.80200000000002</v>
       </c>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="33" t="s">
+      <c r="P16" s="26"/>
+      <c r="Q16" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="R16" s="34"/>
-      <c r="S16" s="34"/>
-      <c r="T16" s="33">
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+      <c r="T16" s="27">
         <v>0.22</v>
       </c>
-      <c r="U16" s="33">
+      <c r="U16" s="27">
         <v>2.5</v>
       </c>
-      <c r="V16" s="35">
+      <c r="V16" s="28">
         <v>20.84</v>
       </c>
       <c r="W16" s="14">
@@ -6212,45 +6343,45 @@
         <f t="shared" si="31"/>
         <v>30</v>
       </c>
-      <c r="AG16" s="31">
+      <c r="AG16" s="25">
         <v>0.1802</v>
       </c>
-      <c r="AH16" s="31">
+      <c r="AH16" s="25">
         <v>0</v>
       </c>
-      <c r="AI16" s="31">
+      <c r="AI16" s="25">
         <v>0.10300000000000001</v>
       </c>
-      <c r="AJ16" s="31">
+      <c r="AJ16" s="25">
         <v>0</v>
       </c>
-      <c r="AK16" s="31">
+      <c r="AK16" s="25">
         <v>5.4000000000000006E-2</v>
       </c>
-      <c r="AL16" s="31">
+      <c r="AL16" s="25">
         <v>0</v>
       </c>
-      <c r="AM16" s="31">
+      <c r="AM16" s="25">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="AN16" s="31">
+      <c r="AN16" s="25">
         <v>0</v>
       </c>
-      <c r="AO16" s="31">
+      <c r="AO16" s="25">
         <v>0.105</v>
       </c>
-      <c r="AP16" s="31">
+      <c r="AP16" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
       <c r="G17" s="1">
         <v>19.66</v>
       </c>
@@ -6270,19 +6401,19 @@
         <f t="shared" si="23"/>
         <v>149.80200000000002</v>
       </c>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="33" t="s">
+      <c r="P17" s="26"/>
+      <c r="Q17" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="R17" s="34"/>
-      <c r="S17" s="34"/>
-      <c r="T17" s="33">
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="27">
         <v>0.3</v>
       </c>
-      <c r="U17" s="33">
+      <c r="U17" s="27">
         <v>10</v>
       </c>
-      <c r="V17" s="35">
+      <c r="V17" s="28">
         <v>19.66</v>
       </c>
       <c r="W17" s="14">
@@ -6317,38 +6448,38 @@
         <f>$U$17*$S$13/$R$13</f>
         <v>30</v>
       </c>
-      <c r="AG17" s="31">
+      <c r="AG17" s="25">
         <v>1.802</v>
       </c>
-      <c r="AH17" s="31">
+      <c r="AH17" s="25">
         <v>4.8262500000000008</v>
       </c>
-      <c r="AI17" s="31">
+      <c r="AI17" s="25">
         <v>1.03</v>
       </c>
-      <c r="AJ17" s="31">
+      <c r="AJ17" s="25">
         <v>4.8262500000000008</v>
       </c>
-      <c r="AK17" s="31">
+      <c r="AK17" s="25">
         <v>0.54</v>
       </c>
-      <c r="AL17" s="31">
+      <c r="AL17" s="25">
         <v>4.8262500000000008</v>
       </c>
-      <c r="AM17" s="31">
+      <c r="AM17" s="25">
         <v>0.71</v>
       </c>
-      <c r="AN17" s="31">
+      <c r="AN17" s="25">
         <v>4.8262500000000008</v>
       </c>
-      <c r="AO17" s="31">
+      <c r="AO17" s="25">
         <v>1.05</v>
       </c>
-      <c r="AP17" s="31">
+      <c r="AP17" s="25">
         <v>4.8262500000000008</v>
       </c>
     </row>
-    <row r="18" spans="2:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
@@ -6370,10 +6501,10 @@
       <c r="Q18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R18" s="16">
+      <c r="R18" s="31">
         <v>4</v>
       </c>
-      <c r="S18" s="16">
+      <c r="S18" s="31">
         <v>14.4</v>
       </c>
       <c r="T18" s="1" t="s">
@@ -6417,38 +6548,38 @@
         <f>$U$22*$S$18/$R$18</f>
         <v>36</v>
       </c>
-      <c r="AG18" s="31">
+      <c r="AG18" s="25">
         <v>3.6040000000000001</v>
       </c>
-      <c r="AH18" s="31">
+      <c r="AH18" s="25">
         <v>10.53</v>
       </c>
-      <c r="AI18" s="31">
+      <c r="AI18" s="25">
         <v>2.06</v>
       </c>
-      <c r="AJ18" s="31">
+      <c r="AJ18" s="25">
         <v>10.53</v>
       </c>
-      <c r="AK18" s="31">
+      <c r="AK18" s="25">
         <v>1.08</v>
       </c>
-      <c r="AL18" s="31">
+      <c r="AL18" s="25">
         <v>10.53</v>
       </c>
-      <c r="AM18" s="31">
+      <c r="AM18" s="25">
         <v>1.42</v>
       </c>
-      <c r="AN18" s="31">
+      <c r="AN18" s="25">
         <v>10.53</v>
       </c>
-      <c r="AO18" s="31">
+      <c r="AO18" s="25">
         <v>2.1</v>
       </c>
-      <c r="AP18" s="31">
+      <c r="AP18" s="25">
         <v>10.53</v>
       </c>
     </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -6458,8 +6589,8 @@
       <c r="Q19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
       <c r="T19" s="1">
         <v>0.01</v>
       </c>
@@ -6501,38 +6632,38 @@
         <f t="shared" ref="AD19:AD22" si="40">$U$22*$S$18/$R$18</f>
         <v>36</v>
       </c>
-      <c r="AG19" s="31">
+      <c r="AG19" s="25">
         <v>10.811999999999999</v>
       </c>
-      <c r="AH19" s="31">
+      <c r="AH19" s="25">
         <v>48.262500000000003</v>
       </c>
-      <c r="AI19" s="31">
+      <c r="AI19" s="25">
         <v>6.1800000000000006</v>
       </c>
-      <c r="AJ19" s="31">
+      <c r="AJ19" s="25">
         <v>48.262500000000003</v>
       </c>
-      <c r="AK19" s="31">
+      <c r="AK19" s="25">
         <v>3.24</v>
       </c>
-      <c r="AL19" s="31">
+      <c r="AL19" s="25">
         <v>48.262500000000003</v>
       </c>
-      <c r="AM19" s="31">
+      <c r="AM19" s="25">
         <v>4.26</v>
       </c>
-      <c r="AN19" s="31">
+      <c r="AN19" s="25">
         <v>48.262500000000003</v>
       </c>
-      <c r="AO19" s="31">
+      <c r="AO19" s="25">
         <v>6.3</v>
       </c>
-      <c r="AP19" s="31">
+      <c r="AP19" s="25">
         <v>48.262500000000003</v>
       </c>
     </row>
-    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -6542,8 +6673,8 @@
       <c r="Q20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
       <c r="T20" s="1">
         <v>0.15</v>
       </c>
@@ -6586,7 +6717,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -6596,8 +6727,8 @@
       <c r="Q21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
       <c r="T21" s="1">
         <v>0.22</v>
       </c>
@@ -6640,7 +6771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -6650,8 +6781,8 @@
       <c r="Q22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R22" s="16"/>
-      <c r="S22" s="16"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
       <c r="T22" s="1">
         <v>0.3</v>
       </c>
@@ -6693,20 +6824,20 @@
         <f t="shared" si="40"/>
         <v>36</v>
       </c>
-      <c r="AG22" s="29" t="s">
+      <c r="AG22" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="AH22" s="29"/>
-      <c r="AI22" s="29"/>
-      <c r="AJ22" s="29"/>
-      <c r="AK22" s="29"/>
-      <c r="AL22" s="29"/>
-      <c r="AM22" s="29"/>
-      <c r="AN22" s="29"/>
-      <c r="AO22" s="29"/>
-      <c r="AP22" s="29"/>
+      <c r="AH22" s="30"/>
+      <c r="AI22" s="30"/>
+      <c r="AJ22" s="30"/>
+      <c r="AK22" s="30"/>
+      <c r="AL22" s="30"/>
+      <c r="AM22" s="30"/>
+      <c r="AN22" s="30"/>
+      <c r="AO22" s="30"/>
+      <c r="AP22" s="30"/>
     </row>
-    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>30</v>
       </c>
@@ -6734,10 +6865,10 @@
       <c r="S23" s="1">
         <v>24</v>
       </c>
-      <c r="T23" s="17" t="s">
+      <c r="T23" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="U23" s="17"/>
+      <c r="U23" s="32"/>
       <c r="V23" s="9"/>
       <c r="W23" s="11"/>
       <c r="X23" s="13"/>
@@ -6747,28 +6878,28 @@
       <c r="AB23" s="11"/>
       <c r="AC23" s="11"/>
       <c r="AD23" s="11"/>
-      <c r="AG23" s="30" t="s">
+      <c r="AG23" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="AH23" s="30"/>
-      <c r="AI23" s="30" t="s">
+      <c r="AH23" s="29"/>
+      <c r="AI23" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="AJ23" s="30"/>
-      <c r="AK23" s="30" t="s">
+      <c r="AJ23" s="29"/>
+      <c r="AK23" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="AL23" s="30"/>
-      <c r="AM23" s="30" t="s">
+      <c r="AL23" s="29"/>
+      <c r="AM23" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="AN23" s="30"/>
-      <c r="AO23" s="30" t="s">
+      <c r="AN23" s="29"/>
+      <c r="AO23" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="AP23" s="30"/>
+      <c r="AP23" s="29"/>
     </row>
-    <row r="24" spans="2:42" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:42" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>31</v>
       </c>
@@ -6796,10 +6927,10 @@
       <c r="S24" s="1">
         <v>36</v>
       </c>
-      <c r="T24" s="17" t="s">
+      <c r="T24" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="U24" s="17"/>
+      <c r="U24" s="32"/>
       <c r="V24" s="9"/>
       <c r="W24" s="11"/>
       <c r="X24" s="13"/>
@@ -6809,51 +6940,51 @@
       <c r="AB24" s="11"/>
       <c r="AC24" s="11"/>
       <c r="AD24" s="11"/>
-      <c r="AG24" s="31" t="s">
+      <c r="AG24" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AH24" s="31" t="s">
+      <c r="AH24" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AI24" s="31" t="s">
+      <c r="AI24" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AJ24" s="31" t="s">
+      <c r="AJ24" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AK24" s="31" t="s">
+      <c r="AK24" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AL24" s="31" t="s">
+      <c r="AL24" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AM24" s="31" t="s">
+      <c r="AM24" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AN24" s="31" t="s">
+      <c r="AN24" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AO24" s="31" t="s">
+      <c r="AO24" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AP24" s="31" t="s">
+      <c r="AP24" s="25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="31">
         <v>5</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="31">
         <v>84.2</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="32" t="s">
         <v>34</v>
       </c>
       <c r="G25" s="1">
@@ -6881,10 +7012,10 @@
       <c r="Q25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R25" s="16">
+      <c r="R25" s="31">
         <v>5</v>
       </c>
-      <c r="S25" s="16">
+      <c r="S25" s="31">
         <v>84.2</v>
       </c>
       <c r="T25" s="1" t="s">
@@ -6928,44 +7059,44 @@
         <f>$U$29*$S$25/$R$25</f>
         <v>168.4</v>
       </c>
-      <c r="AG25" s="31">
+      <c r="AG25" s="25">
         <v>0.17800000000000002</v>
       </c>
-      <c r="AH25" s="31">
+      <c r="AH25" s="25">
         <v>0</v>
       </c>
-      <c r="AI25" s="31">
+      <c r="AI25" s="25">
         <v>0.21300000000000002</v>
       </c>
-      <c r="AJ25" s="31">
+      <c r="AJ25" s="25">
         <v>0</v>
       </c>
-      <c r="AK25" s="31">
+      <c r="AK25" s="25">
         <v>0.19850000000000001</v>
       </c>
-      <c r="AL25" s="31">
+      <c r="AL25" s="25">
         <v>0</v>
       </c>
-      <c r="AM25" s="31">
+      <c r="AM25" s="25">
         <v>0.2084</v>
       </c>
-      <c r="AN25" s="31">
+      <c r="AN25" s="25">
         <v>0</v>
       </c>
-      <c r="AO25" s="31">
+      <c r="AO25" s="25">
         <v>0.1966</v>
       </c>
-      <c r="AP25" s="31">
+      <c r="AP25" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:42" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="17"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
       <c r="G26" s="1">
         <v>17.7</v>
       </c>
@@ -6988,8 +7119,8 @@
       <c r="Q26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
+      <c r="R26" s="31"/>
+      <c r="S26" s="31"/>
       <c r="T26" s="1">
         <v>0.01</v>
       </c>
@@ -7031,44 +7162,44 @@
         <f t="shared" ref="AD26:AD29" si="50">$U$29*$S$25/$R$25</f>
         <v>168.4</v>
       </c>
-      <c r="AG26" s="31">
+      <c r="AG26" s="25">
         <v>2.67</v>
       </c>
-      <c r="AH26" s="31">
+      <c r="AH26" s="25">
         <v>3</v>
       </c>
-      <c r="AI26" s="31">
+      <c r="AI26" s="25">
         <v>3.1949999999999998</v>
       </c>
-      <c r="AJ26" s="31">
+      <c r="AJ26" s="25">
         <v>3</v>
       </c>
-      <c r="AK26" s="31">
+      <c r="AK26" s="25">
         <v>2.9775</v>
       </c>
-      <c r="AL26" s="31">
+      <c r="AL26" s="25">
         <v>3</v>
       </c>
-      <c r="AM26" s="31">
+      <c r="AM26" s="25">
         <v>3.1259999999999999</v>
       </c>
-      <c r="AN26" s="31">
+      <c r="AN26" s="25">
         <v>3</v>
       </c>
-      <c r="AO26" s="31">
+      <c r="AO26" s="25">
         <v>2.9489999999999998</v>
       </c>
-      <c r="AP26" s="31">
+      <c r="AP26" s="25">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:42" x14ac:dyDescent="0.3">
       <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
       <c r="G27" s="1">
         <v>9.01</v>
       </c>
@@ -7091,8 +7222,8 @@
       <c r="Q27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R27" s="16"/>
-      <c r="S27" s="16"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="31"/>
       <c r="T27" s="1">
         <v>0.35</v>
       </c>
@@ -7134,44 +7265,44 @@
         <f t="shared" si="50"/>
         <v>168.4</v>
       </c>
-      <c r="AG27" s="31">
+      <c r="AG27" s="25">
         <v>3.9160000000000004</v>
       </c>
-      <c r="AH27" s="31">
+      <c r="AH27" s="25">
         <v>7.5</v>
       </c>
-      <c r="AI27" s="31">
+      <c r="AI27" s="25">
         <v>4.6859999999999999</v>
       </c>
-      <c r="AJ27" s="31">
+      <c r="AJ27" s="25">
         <v>7.5</v>
       </c>
-      <c r="AK27" s="31">
+      <c r="AK27" s="25">
         <v>4.367</v>
       </c>
-      <c r="AL27" s="31">
+      <c r="AL27" s="25">
         <v>7.5</v>
       </c>
-      <c r="AM27" s="31">
+      <c r="AM27" s="25">
         <v>4.5848000000000004</v>
       </c>
-      <c r="AN27" s="31">
+      <c r="AN27" s="25">
         <v>7.5</v>
       </c>
-      <c r="AO27" s="31">
+      <c r="AO27" s="25">
         <v>4.3251999999999997</v>
       </c>
-      <c r="AP27" s="31">
+      <c r="AP27" s="25">
         <v>7.5</v>
       </c>
     </row>
-    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:42" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="17"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
       <c r="G28" s="1">
         <v>8.8000000000000007</v>
       </c>
@@ -7194,8 +7325,8 @@
       <c r="Q28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R28" s="16"/>
-      <c r="S28" s="16"/>
+      <c r="R28" s="31"/>
+      <c r="S28" s="31"/>
       <c r="T28" s="1">
         <v>0.45</v>
       </c>
@@ -7237,44 +7368,44 @@
         <f t="shared" si="50"/>
         <v>168.4</v>
       </c>
-      <c r="AG28" s="31">
+      <c r="AG28" s="25">
         <v>5.34</v>
       </c>
-      <c r="AH28" s="31">
+      <c r="AH28" s="25">
         <v>30</v>
       </c>
-      <c r="AI28" s="31">
+      <c r="AI28" s="25">
         <v>6.39</v>
       </c>
-      <c r="AJ28" s="31">
+      <c r="AJ28" s="25">
         <v>30</v>
       </c>
-      <c r="AK28" s="31">
+      <c r="AK28" s="25">
         <v>5.9550000000000001</v>
       </c>
-      <c r="AL28" s="31">
+      <c r="AL28" s="25">
         <v>30</v>
       </c>
-      <c r="AM28" s="31">
+      <c r="AM28" s="25">
         <v>6.2519999999999998</v>
       </c>
-      <c r="AN28" s="31">
+      <c r="AN28" s="25">
         <v>30</v>
       </c>
-      <c r="AO28" s="31">
+      <c r="AO28" s="25">
         <v>5.8979999999999997</v>
       </c>
-      <c r="AP28" s="31">
+      <c r="AP28" s="25">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:42" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
       <c r="G29" s="1">
         <v>11.5</v>
       </c>
@@ -7297,8 +7428,8 @@
       <c r="Q29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
+      <c r="R29" s="31"/>
+      <c r="S29" s="31"/>
       <c r="T29" s="1">
         <v>0.57999999999999996</v>
       </c>
@@ -7341,7 +7472,7 @@
         <v>168.4</v>
       </c>
     </row>
-    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>35</v>
       </c>
@@ -7411,7 +7542,7 @@
       <c r="AC30" s="11"/>
       <c r="AD30" s="11"/>
     </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
         <v>37</v>
       </c>
@@ -7479,43 +7610,151 @@
       <c r="AC31" s="11"/>
       <c r="AD31" s="11"/>
     </row>
-    <row r="32" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:42" x14ac:dyDescent="0.3">
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:38" x14ac:dyDescent="0.3">
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:38" x14ac:dyDescent="0.3">
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="5"/>
     </row>
+    <row r="35" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="AF35" s="36"/>
+      <c r="AG35" s="37"/>
+      <c r="AH35" s="37"/>
+      <c r="AI35" s="37"/>
+      <c r="AJ35" s="37"/>
+      <c r="AK35" s="37"/>
+      <c r="AL35" s="38"/>
+    </row>
+    <row r="36" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="AF36" s="39"/>
+      <c r="AG36" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH36" s="40"/>
+      <c r="AI36" s="40"/>
+      <c r="AJ36" s="40"/>
+      <c r="AK36" s="40"/>
+      <c r="AL36" s="41"/>
+    </row>
+    <row r="37" spans="4:38" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="AF37" s="39"/>
+      <c r="AG37" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH37" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI37" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ37" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK37" s="40"/>
+      <c r="AL37" s="41"/>
+    </row>
+    <row r="38" spans="4:38" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AF38" s="39"/>
+      <c r="AG38" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH38" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI38" s="40">
+        <v>30</v>
+      </c>
+      <c r="AJ38" s="40">
+        <v>3</v>
+      </c>
+      <c r="AK38" s="40"/>
+      <c r="AL38" s="41"/>
+    </row>
+    <row r="39" spans="4:38" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q39" s="3"/>
+      <c r="AF39" s="39"/>
+      <c r="AG39" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH39" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI39" s="40">
+        <v>40</v>
+      </c>
+      <c r="AJ39" s="40">
+        <v>4</v>
+      </c>
+      <c r="AK39" s="40"/>
+      <c r="AL39" s="41"/>
+    </row>
+    <row r="40" spans="4:38" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q40" s="3"/>
+      <c r="AF40" s="39"/>
+      <c r="AG40" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH40" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI40" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ40" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK40" s="40"/>
+      <c r="AL40" s="41"/>
+    </row>
+    <row r="41" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="Q41" s="3"/>
+      <c r="AF41" s="39"/>
+      <c r="AG41" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH41" s="43"/>
+      <c r="AI41" s="40"/>
+      <c r="AJ41" s="40"/>
+      <c r="AK41" s="40"/>
+      <c r="AL41" s="41"/>
+    </row>
+    <row r="42" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="AF42" s="44"/>
+      <c r="AG42" s="45"/>
+      <c r="AH42" s="46"/>
+      <c r="AI42" s="45"/>
+      <c r="AJ42" s="45"/>
+      <c r="AK42" s="45"/>
+      <c r="AL42" s="47"/>
+    </row>
+    <row r="43" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="AH43" s="5"/>
+    </row>
+    <row r="44" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="AH44" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="AM14:AN14"/>
-    <mergeCell ref="AO14:AP14"/>
-    <mergeCell ref="AG13:AP13"/>
-    <mergeCell ref="AG2:AP2"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="AM3:AN3"/>
-    <mergeCell ref="AO3:AP3"/>
-    <mergeCell ref="R25:R29"/>
-    <mergeCell ref="S25:S29"/>
-    <mergeCell ref="AG14:AH14"/>
-    <mergeCell ref="AI14:AJ14"/>
-    <mergeCell ref="AK14:AL14"/>
-    <mergeCell ref="AG22:AP22"/>
-    <mergeCell ref="AG23:AH23"/>
-    <mergeCell ref="AI23:AJ23"/>
-    <mergeCell ref="AK23:AL23"/>
-    <mergeCell ref="AM23:AN23"/>
-    <mergeCell ref="AO23:AP23"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="R18:R22"/>
+    <mergeCell ref="S18:S22"/>
+    <mergeCell ref="S3:S7"/>
+    <mergeCell ref="R3:R7"/>
+    <mergeCell ref="R8:R12"/>
+    <mergeCell ref="S8:S12"/>
+    <mergeCell ref="S13:S17"/>
+    <mergeCell ref="R13:R17"/>
     <mergeCell ref="F3:F7"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="D3:D7"/>
@@ -7528,17 +7767,26 @@
     <mergeCell ref="D13:D17"/>
     <mergeCell ref="E13:E17"/>
     <mergeCell ref="F13:F17"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="R18:R22"/>
-    <mergeCell ref="S18:S22"/>
-    <mergeCell ref="S3:S7"/>
-    <mergeCell ref="R3:R7"/>
-    <mergeCell ref="R8:R12"/>
-    <mergeCell ref="S8:S12"/>
-    <mergeCell ref="S13:S17"/>
-    <mergeCell ref="R13:R17"/>
+    <mergeCell ref="R25:R29"/>
+    <mergeCell ref="S25:S29"/>
+    <mergeCell ref="AG14:AH14"/>
+    <mergeCell ref="AI14:AJ14"/>
+    <mergeCell ref="AK14:AL14"/>
+    <mergeCell ref="AG22:AP22"/>
+    <mergeCell ref="AG23:AH23"/>
+    <mergeCell ref="AI23:AJ23"/>
+    <mergeCell ref="AK23:AL23"/>
+    <mergeCell ref="AM23:AN23"/>
+    <mergeCell ref="AO23:AP23"/>
+    <mergeCell ref="AM14:AN14"/>
+    <mergeCell ref="AO14:AP14"/>
+    <mergeCell ref="AG13:AP13"/>
+    <mergeCell ref="AG2:AP2"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AM3:AN3"/>
+    <mergeCell ref="AO3:AP3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>